<commit_message>
[New] Final submission of lit review outline and research matrix
</commit_message>
<xml_diff>
--- a/SEM_2/CS6472-Research_Methods_and_Specification/Research_plan_matrix-23052058.xlsx
+++ b/SEM_2/CS6472-Research_Methods_and_Specification/Research_plan_matrix-23052058.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Research Topic</t>
   </si>
@@ -31,35 +31,7 @@
     <t xml:space="preserve">Research Problem</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">How accurately can a machine learning model classify the staining of </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">tumour </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">in the breast cancer pathology slides in accordance to the Immunohistochemistry (IHC) scoring guidelines?</t>
-    </r>
+    <t xml:space="preserve">How accurately can a machine learning model classify the staining of tumour in the breast cancer pathology slides in accordance to the Immunohistochemistry (IHC) scoring guidelines?</t>
   </si>
   <si>
     <t xml:space="preserve">Research Goals - consider that goals of your research should be interrelated and enable you to solve the problem</t>
@@ -78,6 +50,20 @@
   </si>
   <si>
     <t xml:space="preserve">Write the headings of the papers that possibly you can write based on these goals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- To develop an accurate machine learning model for IHC scoring for the HER2 protein in breast cancer patients.
+- Compare the results and explore if using machine learning models to automate this scoring is reliable and be acceptable by human pathologists given the ramifications of an inaccurate result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- How reliably can machine learning models perform IHC scoring compared to human pathologists? 
+- What features are most informative for HER2 staining classification? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some methods to achieve this would be to use existing pre-trained deep learning/neural network models that can be fine-tuned for classification of tumor pathology slides with the corresponding IHC score.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data collected will be from existing breast cancer patients whose pathology slides will be digitised. These slide images will be used for the training of the model. The data will be anonymised with the ability to identify the patients only with our coordinator from UHL.</t>
   </si>
   <si>
     <t xml:space="preserve">...</t>
@@ -176,10 +162,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -307,7 +294,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,8 +311,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -427,10 +418,10 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.35546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.13"/>
@@ -497,30 +488,38 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+    <row r="4" customFormat="false" ht="161.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
+      <c r="A7" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>